<commit_message>
Modified problem status in SDE Preparation sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="780" yWindow="945" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Coding Round" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -2013,7 +2013,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2023,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3211,77 +3211,77 @@
       <c r="A114" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B114" s="12" t="s">
+      <c r="B114" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C114" s="3" t="s">
-        <v>3</v>
+      <c r="C114" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="21">
       <c r="A115" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B115" s="12" t="s">
+      <c r="B115" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C115" s="3" t="s">
-        <v>3</v>
+      <c r="C115" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="21">
       <c r="A116" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B116" s="12" t="s">
+      <c r="B116" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C116" s="3" t="s">
-        <v>3</v>
+      <c r="C116" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="21">
       <c r="A117" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B117" s="12" t="s">
+      <c r="B117" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="C117" s="3" t="s">
-        <v>3</v>
+      <c r="C117" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="21">
       <c r="A118" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B118" s="12" t="s">
+      <c r="B118" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C118" s="3" t="s">
-        <v>3</v>
+      <c r="C118" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="21">
       <c r="A119" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B119" s="12" t="s">
+      <c r="B119" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="C119" s="3" t="s">
-        <v>3</v>
+      <c r="C119" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="21">
       <c r="A120" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B120" s="12" t="s">
+      <c r="B120" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C120" s="3" t="s">
-        <v>3</v>
+      <c r="C120" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified problem status in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2018,7 +2018,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2028,8 +2028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2596,33 +2596,33 @@
       <c r="A56" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>3</v>
+      <c r="C56" s="9" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="21">
       <c r="A57" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>3</v>
+      <c r="C57" s="9" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="21">
       <c r="A58" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>3</v>
+      <c r="C58" s="9" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified Coin Change problem status in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A401" workbookViewId="0">
+      <selection activeCell="B415" sqref="B415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6409,11 +6409,11 @@
       <c r="A415" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B415" s="10" t="s">
+      <c r="B415" s="16" t="s">
         <v>392</v>
       </c>
-      <c r="C415" s="1" t="s">
-        <v>3</v>
+      <c r="C415" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="416" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified Edit Distance problem status in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A401" workbookViewId="0">
-      <selection activeCell="B415" sqref="B415"/>
+    <sheetView tabSelected="1" topLeftCell="A415" workbookViewId="0">
+      <selection activeCell="B423" sqref="B423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6475,11 +6475,11 @@
       <c r="A421" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B421" s="10" t="s">
+      <c r="B421" s="16" t="s">
         <v>398</v>
       </c>
-      <c r="C421" s="1" t="s">
-        <v>3</v>
+      <c r="C421" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="422" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified Maximize Cuts problem status in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A415" workbookViewId="0">
-      <selection activeCell="B423" sqref="B423"/>
+    <sheetView tabSelected="1" topLeftCell="A420" workbookViewId="0">
+      <selection activeCell="B429" sqref="B429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6541,11 +6541,11 @@
       <c r="A427" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B427" s="10" t="s">
+      <c r="B427" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="C427" s="1" t="s">
-        <v>3</v>
+      <c r="C427" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="428" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified Partition Equal Subset Problem status in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2050,7 +2050,7 @@
   <dimension ref="A1:D492"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A420" workbookViewId="0">
-      <selection activeCell="B429" sqref="B429"/>
+      <selection activeCell="C422" sqref="C422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6486,11 +6486,11 @@
       <c r="A422" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B422" s="10" t="s">
+      <c r="B422" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="C422" s="1" t="s">
-        <v>3</v>
+      <c r="C422" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="423" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified longest common subsequence problem status in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A420" workbookViewId="0">
-      <selection activeCell="C422" sqref="C422"/>
+    <sheetView tabSelected="1" topLeftCell="A422" workbookViewId="0">
+      <selection activeCell="C428" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6552,11 +6552,11 @@
       <c r="A428" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B428" s="10" t="s">
+      <c r="B428" s="16" t="s">
         <v>404</v>
       </c>
-      <c r="C428" s="1" t="s">
-        <v>3</v>
+      <c r="C428" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="429" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified Longest Repeating Subsequence problem status in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A414" workbookViewId="0">
-      <selection activeCell="C416" sqref="C416"/>
+    <sheetView tabSelected="1" topLeftCell="A421" workbookViewId="0">
+      <selection activeCell="C429" sqref="C429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6563,11 +6563,11 @@
       <c r="A429" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B429" s="10" t="s">
+      <c r="B429" s="16" t="s">
         <v>405</v>
       </c>
-      <c r="C429" s="1" t="s">
-        <v>3</v>
+      <c r="C429" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="430" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified Longest Increasing Subsequence problem status in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A421" workbookViewId="0">
-      <selection activeCell="C429" sqref="C429"/>
+    <sheetView tabSelected="1" topLeftCell="A423" workbookViewId="0">
+      <selection activeCell="C430" sqref="C430"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6574,11 +6574,11 @@
       <c r="A430" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B430" s="10" t="s">
+      <c r="B430" s="16" t="s">
         <v>406</v>
       </c>
-      <c r="C430" s="1" t="s">
-        <v>3</v>
+      <c r="C430" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="431" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified Minimum Number Of Jumps problem status in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A423" workbookViewId="0">
-      <selection activeCell="C430" sqref="C430"/>
+    <sheetView tabSelected="1" topLeftCell="A429" workbookViewId="0">
+      <selection activeCell="B443" sqref="B443"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6717,11 +6717,11 @@
       <c r="A443" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B443" s="10" t="s">
+      <c r="B443" s="16" t="s">
         <v>419</v>
       </c>
-      <c r="C443" s="1" t="s">
-        <v>3</v>
+      <c r="C443" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="444" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified Smallest Sum Contiguous Subarray problem status in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A429" workbookViewId="0">
-      <selection activeCell="B443" sqref="B443"/>
+    <sheetView tabSelected="1" topLeftCell="C443" workbookViewId="0">
+      <selection activeCell="H448" sqref="H448"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6750,11 +6750,11 @@
       <c r="A446" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B446" s="10" t="s">
+      <c r="B446" s="16" t="s">
         <v>422</v>
       </c>
-      <c r="C446" s="1" t="s">
-        <v>3</v>
+      <c r="C446" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="447" spans="1:3" ht="21">
@@ -6794,11 +6794,11 @@
       <c r="A450" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B450" s="10" t="s">
+      <c r="B450" s="16" t="s">
         <v>426</v>
       </c>
-      <c r="C450" s="1" t="s">
-        <v>3</v>
+      <c r="C450" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="451" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified Largest Sum Contiguous Subarray problem status in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C443" workbookViewId="0">
-      <selection activeCell="H448" sqref="H448"/>
+    <sheetView tabSelected="1" topLeftCell="B448" workbookViewId="0">
+      <selection activeCell="K449" sqref="K449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6783,11 +6783,11 @@
       <c r="A449" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B449" s="10" t="s">
+      <c r="B449" s="16" t="s">
         <v>425</v>
       </c>
-      <c r="C449" s="1" t="s">
-        <v>3</v>
+      <c r="C449" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="450" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified problem status for Longest Palindromic Subsequence problem in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B448" workbookViewId="0">
-      <selection activeCell="K449" sqref="K449"/>
+    <sheetView tabSelected="1" topLeftCell="A448" workbookViewId="0">
+      <selection activeCell="B454" sqref="B454"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6849,11 +6849,11 @@
       <c r="A455" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B455" s="10" t="s">
+      <c r="B455" s="16" t="s">
         <v>431</v>
       </c>
-      <c r="C455" s="1" t="s">
-        <v>3</v>
+      <c r="C455" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="456" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified Longest Palindromic Substring problem status in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A448" workbookViewId="0">
-      <selection activeCell="B454" sqref="B454"/>
+    <sheetView tabSelected="1" topLeftCell="A450" workbookViewId="0">
+      <selection activeCell="C457" sqref="C457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6871,11 +6871,11 @@
       <c r="A457" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B457" s="10" t="s">
+      <c r="B457" s="16" t="s">
         <v>433</v>
       </c>
-      <c r="C457" s="1" t="s">
-        <v>3</v>
+      <c r="C457" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="458" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified problem status for Count Palindromic Subsequences problem in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A450" workbookViewId="0">
-      <selection activeCell="C457" sqref="C457"/>
+    <sheetView tabSelected="1" topLeftCell="C450" workbookViewId="0">
+      <selection activeCell="C456" sqref="C456"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6860,11 +6860,11 @@
       <c r="A456" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B456" s="10" t="s">
+      <c r="B456" s="16" t="s">
         <v>432</v>
       </c>
-      <c r="C456" s="1" t="s">
-        <v>3</v>
+      <c r="C456" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="457" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified problem status for Implementing a Stack in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C450" workbookViewId="0">
-      <selection activeCell="C456" sqref="C456"/>
+    <sheetView tabSelected="1" topLeftCell="A299" workbookViewId="0">
+      <selection activeCell="B301" activeCellId="1" sqref="C301 B301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5211,11 +5211,11 @@
       <c r="A301" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B301" s="10" t="s">
+      <c r="B301" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="C301" s="1" t="s">
-        <v>3</v>
+      <c r="C301" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="302" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified problem status for Implementing a Queue in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2050,7 +2050,7 @@
   <dimension ref="A1:D492"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A299" workbookViewId="0">
-      <selection activeCell="B301" activeCellId="1" sqref="C301 B301"/>
+      <selection activeCell="B303" sqref="B303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5222,11 +5222,11 @@
       <c r="A302" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B302" s="10" t="s">
+      <c r="B302" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="C302" s="1" t="s">
-        <v>3</v>
+      <c r="C302" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="303" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified problem status for Reverse A String using Stack problem in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B302" workbookViewId="0">
-      <selection activeCell="B306" sqref="B306"/>
+    <sheetView tabSelected="1" topLeftCell="A302" workbookViewId="0">
+      <selection activeCell="C307" sqref="C307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5277,11 +5277,11 @@
       <c r="A307" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B307" s="10" t="s">
+      <c r="B307" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="C307" s="1" t="s">
-        <v>3</v>
+      <c r="C307" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified problem status for Next Greater Element problem in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A302" workbookViewId="0">
-      <selection activeCell="C307" sqref="C307"/>
+    <sheetView tabSelected="1" topLeftCell="A466" workbookViewId="0">
+      <selection activeCell="B468" sqref="B468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5299,11 +5299,11 @@
       <c r="A309" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B309" s="10" t="s">
+      <c r="B309" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="C309" s="1" t="s">
-        <v>3</v>
+      <c r="C309" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="310" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified problem status for Special Stack problem in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A466" workbookViewId="0">
-      <selection activeCell="B468" sqref="B468"/>
+    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
+      <selection activeCell="C308" sqref="C308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5288,11 +5288,11 @@
       <c r="A308" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B308" s="10" t="s">
+      <c r="B308" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="C308" s="1" t="s">
-        <v>3</v>
+      <c r="C308" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="309" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified problem status for Merge Overlapping Intervals problem in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
-      <selection activeCell="C308" sqref="C308"/>
+    <sheetView tabSelected="1" topLeftCell="B309" workbookViewId="0">
+      <selection activeCell="B316" sqref="B316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5376,11 +5376,11 @@
       <c r="A316" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B316" s="10" t="s">
+      <c r="B316" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="C316" s="1" t="s">
-        <v>3</v>
+      <c r="C316" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="317" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified problem status for Largest Area In A Rectangular Histogram problem in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B309" workbookViewId="0">
-      <selection activeCell="B316" sqref="B316"/>
+    <sheetView tabSelected="1" topLeftCell="B312" workbookViewId="0">
+      <selection activeCell="C317" sqref="C317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5387,11 +5387,11 @@
       <c r="A317" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B317" s="10" t="s">
+      <c r="B317" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="C317" s="1" t="s">
-        <v>3</v>
+      <c r="C317" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified problem status for Celebrity Problem in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B312" workbookViewId="0">
-      <selection activeCell="C317" sqref="C317"/>
+    <sheetView tabSelected="1" topLeftCell="C305" workbookViewId="0">
+      <selection activeCell="C310" sqref="C310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5310,11 +5310,11 @@
       <c r="A310" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B310" s="10" t="s">
+      <c r="B310" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="C310" s="1" t="s">
-        <v>3</v>
+      <c r="C310" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="311" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified problem status for Next Smallest Element problem in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C305" workbookViewId="0">
-      <selection activeCell="C310" sqref="C310"/>
+    <sheetView tabSelected="1" topLeftCell="A332" workbookViewId="0">
+      <selection activeCell="C338" sqref="C338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5618,11 +5618,11 @@
       <c r="A338" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B338" s="10" t="s">
+      <c r="B338" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="C338" s="1" t="s">
-        <v>3</v>
+      <c r="C338" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="339" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Modified problem status for LRU Cache Implementation problem in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -989,9 +989,6 @@
     <t>Implement a Circular queue</t>
   </si>
   <si>
-    <t>LRU Cache Implementationa</t>
-  </si>
-  <si>
     <t>Reverse a Queue using recursion</t>
   </si>
   <si>
@@ -1473,6 +1470,9 @@
   </si>
   <si>
     <t>Why strings are immutable in Javascript?</t>
+  </si>
+  <si>
+    <t>LRU Cache Implementation</t>
   </si>
 </sst>
 </file>
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A332" workbookViewId="0">
-      <selection activeCell="C338" sqref="C338"/>
+    <sheetView tabSelected="1" topLeftCell="C319" workbookViewId="0">
+      <selection activeCell="C326" sqref="C326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2063,7 +2063,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="6" customFormat="1" ht="45" customHeight="1">
       <c r="B1" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2080,7 +2080,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2094,7 +2094,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21">
@@ -2105,7 +2105,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21">
@@ -2116,7 +2116,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21">
@@ -2127,7 +2127,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="21">
@@ -2138,7 +2138,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21">
@@ -2149,7 +2149,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="21">
@@ -2160,7 +2160,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="21">
@@ -2171,7 +2171,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="21">
@@ -2182,7 +2182,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21">
@@ -2193,7 +2193,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="21">
@@ -2204,7 +2204,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21">
@@ -2215,7 +2215,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21">
@@ -2226,7 +2226,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21">
@@ -2237,7 +2237,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21">
@@ -2248,7 +2248,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21">
@@ -2259,7 +2259,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="21">
@@ -2270,7 +2270,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21">
@@ -2281,7 +2281,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21">
@@ -2292,7 +2292,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="21">
@@ -2303,7 +2303,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="21">
@@ -2621,7 +2621,7 @@
         <v>53</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="21">
@@ -2632,7 +2632,7 @@
         <v>54</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="21">
@@ -2643,7 +2643,7 @@
         <v>55</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="21">
@@ -2651,10 +2651,10 @@
         <v>52</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="21">
@@ -2665,7 +2665,7 @@
         <v>56</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="21">
@@ -2676,7 +2676,7 @@
         <v>57</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="21">
@@ -2698,7 +2698,7 @@
         <v>59</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="21">
@@ -2720,7 +2720,7 @@
         <v>61</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="21">
@@ -2731,7 +2731,7 @@
         <v>62</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="21">
@@ -2742,7 +2742,7 @@
         <v>63</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="21">
@@ -2753,7 +2753,7 @@
         <v>64</v>
       </c>
       <c r="C68" s="23" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="21">
@@ -3102,7 +3102,7 @@
         <v>96</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="21">
@@ -3113,7 +3113,7 @@
         <v>97</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="21">
@@ -3124,7 +3124,7 @@
         <v>98</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="21">
@@ -3135,7 +3135,7 @@
         <v>99</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="21">
@@ -3168,7 +3168,7 @@
         <v>102</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="21">
@@ -3176,13 +3176,13 @@
         <v>95</v>
       </c>
       <c r="B108" s="16" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="21">
@@ -3190,10 +3190,10 @@
         <v>95</v>
       </c>
       <c r="B109" s="16" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="21">
@@ -3204,7 +3204,7 @@
         <v>103</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="21">
@@ -3212,10 +3212,10 @@
         <v>95</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="21">
@@ -3223,10 +3223,10 @@
         <v>95</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="21">
@@ -3234,7 +3234,7 @@
         <v>95</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>3</v>
@@ -3248,7 +3248,7 @@
         <v>104</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="21">
@@ -3259,7 +3259,7 @@
         <v>105</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="21">
@@ -3270,7 +3270,7 @@
         <v>106</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="21">
@@ -3281,7 +3281,7 @@
         <v>107</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="21">
@@ -3292,7 +3292,7 @@
         <v>108</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="21">
@@ -3303,7 +3303,7 @@
         <v>109</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="21">
@@ -3314,7 +3314,7 @@
         <v>110</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="21">
@@ -3560,7 +3560,7 @@
         <v>133</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="21">
@@ -3571,7 +3571,7 @@
         <v>134</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="21">
@@ -3582,7 +3582,7 @@
         <v>135</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="21">
@@ -3593,7 +3593,7 @@
         <v>136</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="21">
@@ -3604,7 +3604,7 @@
         <v>137</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="21">
@@ -3615,7 +3615,7 @@
         <v>138</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="21">
@@ -3626,7 +3626,7 @@
         <v>139</v>
       </c>
       <c r="C150" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="21">
@@ -3637,7 +3637,7 @@
         <v>140</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="21">
@@ -3648,7 +3648,7 @@
         <v>141</v>
       </c>
       <c r="C152" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="21">
@@ -3659,7 +3659,7 @@
         <v>142</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="21">
@@ -3670,7 +3670,7 @@
         <v>143</v>
       </c>
       <c r="C154" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="21">
@@ -3681,7 +3681,7 @@
         <v>144</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="21">
@@ -3714,7 +3714,7 @@
         <v>147</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="21">
@@ -3725,7 +3725,7 @@
         <v>148</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="21">
@@ -3747,7 +3747,7 @@
         <v>150</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="21">
@@ -3758,7 +3758,7 @@
         <v>151</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="21">
@@ -3769,7 +3769,7 @@
         <v>152</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="21">
@@ -3780,7 +3780,7 @@
         <v>153</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="21">
@@ -5215,7 +5215,7 @@
         <v>284</v>
       </c>
       <c r="C301" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="302" spans="1:3" ht="21">
@@ -5226,7 +5226,7 @@
         <v>285</v>
       </c>
       <c r="C302" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="303" spans="1:3" ht="21">
@@ -5237,7 +5237,7 @@
         <v>286</v>
       </c>
       <c r="C303" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="304" spans="1:3" ht="21">
@@ -5270,7 +5270,7 @@
         <v>289</v>
       </c>
       <c r="C306" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="307" spans="1:3" ht="21">
@@ -5281,7 +5281,7 @@
         <v>290</v>
       </c>
       <c r="C307" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="21">
@@ -5292,7 +5292,7 @@
         <v>291</v>
       </c>
       <c r="C308" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="309" spans="1:3" ht="21">
@@ -5303,7 +5303,7 @@
         <v>292</v>
       </c>
       <c r="C309" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="310" spans="1:3" ht="21">
@@ -5314,7 +5314,7 @@
         <v>293</v>
       </c>
       <c r="C310" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="311" spans="1:3" ht="21">
@@ -5380,7 +5380,7 @@
         <v>299</v>
       </c>
       <c r="C316" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="317" spans="1:3" ht="21">
@@ -5391,7 +5391,7 @@
         <v>300</v>
       </c>
       <c r="C317" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="21">
@@ -5486,11 +5486,11 @@
       <c r="A326" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B326" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="C326" s="1" t="s">
-        <v>3</v>
+      <c r="B326" s="16" t="s">
+        <v>470</v>
+      </c>
+      <c r="C326" s="8" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="327" spans="1:3" ht="21">
@@ -5498,7 +5498,7 @@
         <v>283</v>
       </c>
       <c r="B327" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C327" s="1" t="s">
         <v>3</v>
@@ -5509,7 +5509,7 @@
         <v>283</v>
       </c>
       <c r="B328" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C328" s="1" t="s">
         <v>3</v>
@@ -5520,7 +5520,7 @@
         <v>283</v>
       </c>
       <c r="B329" s="10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C329" s="1" t="s">
         <v>3</v>
@@ -5531,7 +5531,7 @@
         <v>283</v>
       </c>
       <c r="B330" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C330" s="1" t="s">
         <v>3</v>
@@ -5542,7 +5542,7 @@
         <v>283</v>
       </c>
       <c r="B331" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C331" s="1" t="s">
         <v>3</v>
@@ -5553,7 +5553,7 @@
         <v>283</v>
       </c>
       <c r="B332" s="10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C332" s="1" t="s">
         <v>3</v>
@@ -5564,7 +5564,7 @@
         <v>283</v>
       </c>
       <c r="B333" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C333" s="1" t="s">
         <v>3</v>
@@ -5575,7 +5575,7 @@
         <v>283</v>
       </c>
       <c r="B334" s="10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C334" s="1" t="s">
         <v>3</v>
@@ -5586,7 +5586,7 @@
         <v>283</v>
       </c>
       <c r="B335" s="10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C335" s="1" t="s">
         <v>3</v>
@@ -5597,7 +5597,7 @@
         <v>283</v>
       </c>
       <c r="B336" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C336" s="1" t="s">
         <v>3</v>
@@ -5608,7 +5608,7 @@
         <v>283</v>
       </c>
       <c r="B337" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C337" s="1" t="s">
         <v>3</v>
@@ -5619,10 +5619,10 @@
         <v>283</v>
       </c>
       <c r="B338" s="16" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C338" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="339" spans="1:3" ht="21">
@@ -5635,10 +5635,10 @@
     </row>
     <row r="341" spans="1:3" ht="21">
       <c r="A341" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B341" s="10" t="s">
         <v>322</v>
-      </c>
-      <c r="B341" s="10" t="s">
-        <v>323</v>
       </c>
       <c r="C341" s="1" t="s">
         <v>3</v>
@@ -5646,10 +5646,10 @@
     </row>
     <row r="342" spans="1:3" ht="21">
       <c r="A342" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B342" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C342" s="1" t="s">
         <v>3</v>
@@ -5657,10 +5657,10 @@
     </row>
     <row r="343" spans="1:3" ht="21">
       <c r="A343" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B343" s="10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C343" s="1" t="s">
         <v>3</v>
@@ -5668,10 +5668,10 @@
     </row>
     <row r="344" spans="1:3" ht="21">
       <c r="A344" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B344" s="10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C344" s="1" t="s">
         <v>3</v>
@@ -5679,10 +5679,10 @@
     </row>
     <row r="345" spans="1:3" ht="21">
       <c r="A345" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B345" s="10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C345" s="1" t="s">
         <v>3</v>
@@ -5690,10 +5690,10 @@
     </row>
     <row r="346" spans="1:3" ht="21">
       <c r="A346" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B346" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C346" s="1" t="s">
         <v>3</v>
@@ -5701,10 +5701,10 @@
     </row>
     <row r="347" spans="1:3" ht="21">
       <c r="A347" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B347" s="10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C347" s="1" t="s">
         <v>3</v>
@@ -5712,10 +5712,10 @@
     </row>
     <row r="348" spans="1:3" ht="21">
       <c r="A348" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B348" s="10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C348" s="1" t="s">
         <v>3</v>
@@ -5723,10 +5723,10 @@
     </row>
     <row r="349" spans="1:3" ht="21">
       <c r="A349" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B349" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C349" s="1" t="s">
         <v>3</v>
@@ -5734,10 +5734,10 @@
     </row>
     <row r="350" spans="1:3" ht="21">
       <c r="A350" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B350" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C350" s="1" t="s">
         <v>3</v>
@@ -5745,10 +5745,10 @@
     </row>
     <row r="351" spans="1:3" ht="21">
       <c r="A351" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B351" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C351" s="1" t="s">
         <v>3</v>
@@ -5756,10 +5756,10 @@
     </row>
     <row r="352" spans="1:3" ht="21">
       <c r="A352" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B352" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C352" s="1" t="s">
         <v>3</v>
@@ -5767,10 +5767,10 @@
     </row>
     <row r="353" spans="1:3" ht="21">
       <c r="A353" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B353" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C353" s="1" t="s">
         <v>3</v>
@@ -5778,10 +5778,10 @@
     </row>
     <row r="354" spans="1:3" ht="21">
       <c r="A354" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B354" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C354" s="1" t="s">
         <v>3</v>
@@ -5789,10 +5789,10 @@
     </row>
     <row r="355" spans="1:3" ht="21">
       <c r="A355" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B355" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C355" s="1" t="s">
         <v>3</v>
@@ -5800,10 +5800,10 @@
     </row>
     <row r="356" spans="1:3" ht="21">
       <c r="A356" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B356" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C356" s="1" t="s">
         <v>3</v>
@@ -5811,10 +5811,10 @@
     </row>
     <row r="357" spans="1:3" ht="21">
       <c r="A357" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B357" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C357" s="1" t="s">
         <v>3</v>
@@ -5822,10 +5822,10 @@
     </row>
     <row r="358" spans="1:3" ht="21">
       <c r="A358" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B358" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C358" s="1" t="s">
         <v>3</v>
@@ -5841,10 +5841,10 @@
     </row>
     <row r="361" spans="1:3" ht="21">
       <c r="A361" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B361" s="10" t="s">
         <v>341</v>
-      </c>
-      <c r="B361" s="10" t="s">
-        <v>342</v>
       </c>
       <c r="C361" s="1" t="s">
         <v>3</v>
@@ -5852,10 +5852,10 @@
     </row>
     <row r="362" spans="1:3" ht="21">
       <c r="A362" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B362" s="10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C362" s="1" t="s">
         <v>3</v>
@@ -5863,10 +5863,10 @@
     </row>
     <row r="363" spans="1:3" ht="21">
       <c r="A363" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B363" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C363" s="1" t="s">
         <v>3</v>
@@ -5874,10 +5874,10 @@
     </row>
     <row r="364" spans="1:3" ht="21">
       <c r="A364" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B364" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C364" s="1" t="s">
         <v>3</v>
@@ -5885,10 +5885,10 @@
     </row>
     <row r="365" spans="1:3" ht="21">
       <c r="A365" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B365" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C365" s="1" t="s">
         <v>3</v>
@@ -5896,10 +5896,10 @@
     </row>
     <row r="366" spans="1:3" ht="21">
       <c r="A366" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B366" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C366" s="1" t="s">
         <v>3</v>
@@ -5907,10 +5907,10 @@
     </row>
     <row r="367" spans="1:3" ht="21">
       <c r="A367" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B367" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C367" s="1" t="s">
         <v>3</v>
@@ -5918,10 +5918,10 @@
     </row>
     <row r="368" spans="1:3" ht="21">
       <c r="A368" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B368" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C368" s="1" t="s">
         <v>3</v>
@@ -5929,10 +5929,10 @@
     </row>
     <row r="369" spans="1:3" ht="21">
       <c r="A369" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B369" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C369" s="1" t="s">
         <v>3</v>
@@ -5940,10 +5940,10 @@
     </row>
     <row r="370" spans="1:3" ht="21">
       <c r="A370" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B370" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C370" s="1" t="s">
         <v>3</v>
@@ -5951,10 +5951,10 @@
     </row>
     <row r="371" spans="1:3" ht="21">
       <c r="A371" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B371" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C371" s="1" t="s">
         <v>3</v>
@@ -5962,10 +5962,10 @@
     </row>
     <row r="372" spans="1:3" ht="21">
       <c r="A372" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B372" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C372" s="1" t="s">
         <v>3</v>
@@ -5973,10 +5973,10 @@
     </row>
     <row r="373" spans="1:3" ht="21">
       <c r="A373" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B373" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C373" s="1" t="s">
         <v>3</v>
@@ -5984,10 +5984,10 @@
     </row>
     <row r="374" spans="1:3" ht="21">
       <c r="A374" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B374" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C374" s="1" t="s">
         <v>3</v>
@@ -5995,10 +5995,10 @@
     </row>
     <row r="375" spans="1:3" ht="21">
       <c r="A375" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B375" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C375" s="1" t="s">
         <v>3</v>
@@ -6006,10 +6006,10 @@
     </row>
     <row r="376" spans="1:3" ht="21">
       <c r="A376" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B376" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C376" s="1" t="s">
         <v>3</v>
@@ -6017,10 +6017,10 @@
     </row>
     <row r="377" spans="1:3" ht="21">
       <c r="A377" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B377" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C377" s="1" t="s">
         <v>3</v>
@@ -6028,10 +6028,10 @@
     </row>
     <row r="378" spans="1:3" ht="21">
       <c r="A378" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B378" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C378" s="1" t="s">
         <v>3</v>
@@ -6039,10 +6039,10 @@
     </row>
     <row r="379" spans="1:3" ht="21">
       <c r="A379" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B379" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C379" s="1" t="s">
         <v>3</v>
@@ -6050,10 +6050,10 @@
     </row>
     <row r="380" spans="1:3" ht="21">
       <c r="A380" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B380" s="10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C380" s="1" t="s">
         <v>3</v>
@@ -6061,10 +6061,10 @@
     </row>
     <row r="381" spans="1:3" ht="21">
       <c r="A381" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B381" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C381" s="1" t="s">
         <v>3</v>
@@ -6072,10 +6072,10 @@
     </row>
     <row r="382" spans="1:3" ht="21">
       <c r="A382" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B382" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C382" s="1" t="s">
         <v>3</v>
@@ -6083,10 +6083,10 @@
     </row>
     <row r="383" spans="1:3" ht="21">
       <c r="A383" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B383" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C383" s="1" t="s">
         <v>3</v>
@@ -6094,10 +6094,10 @@
     </row>
     <row r="384" spans="1:3" ht="21">
       <c r="A384" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B384" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C384" s="1" t="s">
         <v>3</v>
@@ -6105,10 +6105,10 @@
     </row>
     <row r="385" spans="1:3" ht="21">
       <c r="A385" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B385" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C385" s="1" t="s">
         <v>3</v>
@@ -6116,10 +6116,10 @@
     </row>
     <row r="386" spans="1:3" ht="21">
       <c r="A386" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B386" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C386" s="1" t="s">
         <v>3</v>
@@ -6127,10 +6127,10 @@
     </row>
     <row r="387" spans="1:3" ht="21">
       <c r="A387" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B387" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C387" s="1" t="s">
         <v>3</v>
@@ -6138,10 +6138,10 @@
     </row>
     <row r="388" spans="1:3" ht="21">
       <c r="A388" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B388" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C388" s="1" t="s">
         <v>3</v>
@@ -6149,10 +6149,10 @@
     </row>
     <row r="389" spans="1:3" ht="21">
       <c r="A389" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B389" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C389" s="1" t="s">
         <v>3</v>
@@ -6160,10 +6160,10 @@
     </row>
     <row r="390" spans="1:3" ht="21">
       <c r="A390" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B390" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C390" s="1" t="s">
         <v>3</v>
@@ -6171,10 +6171,10 @@
     </row>
     <row r="391" spans="1:3" ht="21">
       <c r="A391" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B391" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C391" s="1" t="s">
         <v>3</v>
@@ -6182,10 +6182,10 @@
     </row>
     <row r="392" spans="1:3" ht="21">
       <c r="A392" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B392" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C392" s="1" t="s">
         <v>3</v>
@@ -6193,10 +6193,10 @@
     </row>
     <row r="393" spans="1:3" ht="21">
       <c r="A393" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B393" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C393" s="1" t="s">
         <v>3</v>
@@ -6204,10 +6204,10 @@
     </row>
     <row r="394" spans="1:3" ht="21">
       <c r="A394" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B394" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C394" s="1" t="s">
         <v>3</v>
@@ -6215,10 +6215,10 @@
     </row>
     <row r="395" spans="1:3" ht="21">
       <c r="A395" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B395" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C395" s="1" t="s">
         <v>3</v>
@@ -6226,10 +6226,10 @@
     </row>
     <row r="396" spans="1:3" ht="21">
       <c r="A396" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B396" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C396" s="1" t="s">
         <v>3</v>
@@ -6237,10 +6237,10 @@
     </row>
     <row r="397" spans="1:3" ht="21">
       <c r="A397" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B397" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C397" s="1" t="s">
         <v>3</v>
@@ -6248,10 +6248,10 @@
     </row>
     <row r="398" spans="1:3" ht="21">
       <c r="A398" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B398" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C398" s="1" t="s">
         <v>3</v>
@@ -6259,10 +6259,10 @@
     </row>
     <row r="399" spans="1:3" ht="21">
       <c r="A399" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B399" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C399" s="1" t="s">
         <v>3</v>
@@ -6270,10 +6270,10 @@
     </row>
     <row r="400" spans="1:3" ht="21">
       <c r="A400" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B400" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C400" s="1" t="s">
         <v>3</v>
@@ -6281,10 +6281,10 @@
     </row>
     <row r="401" spans="1:3" ht="21">
       <c r="A401" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B401" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C401" s="1" t="s">
         <v>3</v>
@@ -6292,10 +6292,10 @@
     </row>
     <row r="402" spans="1:3" ht="21">
       <c r="A402" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B402" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C402" s="1" t="s">
         <v>3</v>
@@ -6303,10 +6303,10 @@
     </row>
     <row r="403" spans="1:3" ht="21">
       <c r="A403" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B403" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C403" s="1" t="s">
         <v>3</v>
@@ -6314,10 +6314,10 @@
     </row>
     <row r="404" spans="1:3" ht="21">
       <c r="A404" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B404" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C404" s="1" t="s">
         <v>3</v>
@@ -6333,10 +6333,10 @@
     </row>
     <row r="407" spans="1:3" ht="21">
       <c r="A407" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B407" s="10" t="s">
         <v>385</v>
-      </c>
-      <c r="B407" s="10" t="s">
-        <v>386</v>
       </c>
       <c r="C407" s="1" t="s">
         <v>3</v>
@@ -6344,10 +6344,10 @@
     </row>
     <row r="408" spans="1:3" ht="21">
       <c r="A408" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B408" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C408" s="1" t="s">
         <v>3</v>
@@ -6355,10 +6355,10 @@
     </row>
     <row r="409" spans="1:3" ht="21">
       <c r="A409" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B409" s="10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C409" s="1" t="s">
         <v>3</v>
@@ -6366,7 +6366,7 @@
     </row>
     <row r="410" spans="1:3" ht="21">
       <c r="A410" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B410" s="10" t="s">
         <v>87</v>
@@ -6377,10 +6377,10 @@
     </row>
     <row r="411" spans="1:3" ht="21">
       <c r="A411" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B411" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C411" s="1" t="s">
         <v>3</v>
@@ -6388,10 +6388,10 @@
     </row>
     <row r="412" spans="1:3" ht="21">
       <c r="A412" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B412" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C412" s="1" t="s">
         <v>3</v>
@@ -6407,32 +6407,32 @@
     </row>
     <row r="415" spans="1:3" ht="21">
       <c r="A415" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B415" s="16" t="s">
         <v>391</v>
       </c>
-      <c r="B415" s="16" t="s">
-        <v>392</v>
-      </c>
       <c r="C415" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="416" spans="1:3" ht="21">
       <c r="A416" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B416" s="16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C416" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="417" spans="1:3" ht="21">
       <c r="A417" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B417" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C417" s="1" t="s">
         <v>3</v>
@@ -6440,10 +6440,10 @@
     </row>
     <row r="418" spans="1:3" ht="21">
       <c r="A418" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B418" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C418" s="1" t="s">
         <v>3</v>
@@ -6451,10 +6451,10 @@
     </row>
     <row r="419" spans="1:3" ht="21">
       <c r="A419" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B419" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C419" s="1" t="s">
         <v>3</v>
@@ -6462,10 +6462,10 @@
     </row>
     <row r="420" spans="1:3" ht="21">
       <c r="A420" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B420" s="10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C420" s="1" t="s">
         <v>3</v>
@@ -6473,32 +6473,32 @@
     </row>
     <row r="421" spans="1:3" ht="21">
       <c r="A421" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B421" s="16" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C421" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="422" spans="1:3" ht="21">
       <c r="A422" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B422" s="16" t="s">
         <v>271</v>
       </c>
       <c r="C422" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="423" spans="1:3" ht="21">
       <c r="A423" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B423" s="10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C423" s="1" t="s">
         <v>3</v>
@@ -6506,10 +6506,10 @@
     </row>
     <row r="424" spans="1:3" ht="21">
       <c r="A424" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B424" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C424" s="1" t="s">
         <v>3</v>
@@ -6517,10 +6517,10 @@
     </row>
     <row r="425" spans="1:3" ht="21">
       <c r="A425" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B425" s="10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C425" s="1" t="s">
         <v>3</v>
@@ -6528,10 +6528,10 @@
     </row>
     <row r="426" spans="1:3" ht="21">
       <c r="A426" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B426" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C426" s="1" t="s">
         <v>3</v>
@@ -6539,54 +6539,54 @@
     </row>
     <row r="427" spans="1:3" ht="21">
       <c r="A427" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B427" s="16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C427" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="428" spans="1:3" ht="21">
       <c r="A428" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B428" s="16" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C428" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="429" spans="1:3" ht="21">
       <c r="A429" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B429" s="16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C429" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="430" spans="1:3" ht="21">
       <c r="A430" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B430" s="16" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C430" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="431" spans="1:3" ht="21">
       <c r="A431" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B431" s="10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C431" s="1" t="s">
         <v>3</v>
@@ -6594,10 +6594,10 @@
     </row>
     <row r="432" spans="1:3" ht="21">
       <c r="A432" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B432" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C432" s="1" t="s">
         <v>3</v>
@@ -6605,10 +6605,10 @@
     </row>
     <row r="433" spans="1:3" ht="21">
       <c r="A433" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B433" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C433" s="1" t="s">
         <v>3</v>
@@ -6616,10 +6616,10 @@
     </row>
     <row r="434" spans="1:3" ht="21">
       <c r="A434" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B434" s="10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C434" s="1" t="s">
         <v>3</v>
@@ -6627,10 +6627,10 @@
     </row>
     <row r="435" spans="1:3" ht="21">
       <c r="A435" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B435" s="10" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C435" s="1" t="s">
         <v>3</v>
@@ -6638,10 +6638,10 @@
     </row>
     <row r="436" spans="1:3" ht="21">
       <c r="A436" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B436" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C436" s="1" t="s">
         <v>3</v>
@@ -6649,10 +6649,10 @@
     </row>
     <row r="437" spans="1:3" ht="21">
       <c r="A437" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B437" s="10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C437" s="1" t="s">
         <v>3</v>
@@ -6660,10 +6660,10 @@
     </row>
     <row r="438" spans="1:3" ht="21">
       <c r="A438" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B438" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C438" s="1" t="s">
         <v>3</v>
@@ -6671,10 +6671,10 @@
     </row>
     <row r="439" spans="1:3" ht="21">
       <c r="A439" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B439" s="10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C439" s="1" t="s">
         <v>3</v>
@@ -6682,10 +6682,10 @@
     </row>
     <row r="440" spans="1:3" ht="21">
       <c r="A440" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B440" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C440" s="1" t="s">
         <v>3</v>
@@ -6693,10 +6693,10 @@
     </row>
     <row r="441" spans="1:3" ht="21">
       <c r="A441" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B441" s="10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C441" s="1" t="s">
         <v>3</v>
@@ -6704,10 +6704,10 @@
     </row>
     <row r="442" spans="1:3" ht="21">
       <c r="A442" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B442" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C442" s="1" t="s">
         <v>3</v>
@@ -6715,21 +6715,21 @@
     </row>
     <row r="443" spans="1:3" ht="21">
       <c r="A443" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B443" s="16" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C443" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="444" spans="1:3" ht="21">
       <c r="A444" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B444" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C444" s="1" t="s">
         <v>3</v>
@@ -6737,10 +6737,10 @@
     </row>
     <row r="445" spans="1:3" ht="21">
       <c r="A445" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B445" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C445" s="1" t="s">
         <v>3</v>
@@ -6748,21 +6748,21 @@
     </row>
     <row r="446" spans="1:3" ht="21">
       <c r="A446" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B446" s="16" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C446" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="447" spans="1:3" ht="21">
       <c r="A447" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B447" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C447" s="1" t="s">
         <v>3</v>
@@ -6770,10 +6770,10 @@
     </row>
     <row r="448" spans="1:3" ht="21">
       <c r="A448" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B448" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C448" s="1" t="s">
         <v>3</v>
@@ -6781,32 +6781,32 @@
     </row>
     <row r="449" spans="1:3" ht="21">
       <c r="A449" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B449" s="16" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C449" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="450" spans="1:3" ht="21">
       <c r="A450" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B450" s="16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C450" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="451" spans="1:3" ht="21">
       <c r="A451" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B451" s="10" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C451" s="1" t="s">
         <v>3</v>
@@ -6814,10 +6814,10 @@
     </row>
     <row r="452" spans="1:3" ht="21">
       <c r="A452" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B452" s="10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C452" s="1" t="s">
         <v>3</v>
@@ -6825,10 +6825,10 @@
     </row>
     <row r="453" spans="1:3" ht="21">
       <c r="A453" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B453" s="10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C453" s="1" t="s">
         <v>3</v>
@@ -6836,10 +6836,10 @@
     </row>
     <row r="454" spans="1:3" ht="21">
       <c r="A454" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B454" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C454" s="1" t="s">
         <v>3</v>
@@ -6847,43 +6847,43 @@
     </row>
     <row r="455" spans="1:3" ht="21">
       <c r="A455" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B455" s="16" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C455" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="456" spans="1:3" ht="21">
       <c r="A456" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B456" s="16" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C456" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="457" spans="1:3" ht="21">
       <c r="A457" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B457" s="16" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C457" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="458" spans="1:3" ht="21">
       <c r="A458" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B458" s="10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C458" s="1" t="s">
         <v>3</v>
@@ -6891,10 +6891,10 @@
     </row>
     <row r="459" spans="1:3" ht="21">
       <c r="A459" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B459" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C459" s="1" t="s">
         <v>3</v>
@@ -6902,10 +6902,10 @@
     </row>
     <row r="460" spans="1:3" ht="21">
       <c r="A460" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B460" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C460" s="1" t="s">
         <v>3</v>
@@ -6913,10 +6913,10 @@
     </row>
     <row r="461" spans="1:3" ht="21">
       <c r="A461" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B461" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C461" s="1" t="s">
         <v>3</v>
@@ -6924,10 +6924,10 @@
     </row>
     <row r="462" spans="1:3" ht="21">
       <c r="A462" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B462" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C462" s="1" t="s">
         <v>3</v>
@@ -6935,10 +6935,10 @@
     </row>
     <row r="463" spans="1:3" ht="21">
       <c r="A463" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B463" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C463" s="1" t="s">
         <v>3</v>
@@ -6946,10 +6946,10 @@
     </row>
     <row r="464" spans="1:3" ht="21">
       <c r="A464" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B464" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C464" s="1" t="s">
         <v>3</v>
@@ -6957,10 +6957,10 @@
     </row>
     <row r="465" spans="1:3" ht="21">
       <c r="A465" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B465" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C465" s="1" t="s">
         <v>3</v>
@@ -6968,10 +6968,10 @@
     </row>
     <row r="466" spans="1:3" ht="21">
       <c r="A466" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B466" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C466" s="1" t="s">
         <v>3</v>
@@ -6979,10 +6979,10 @@
     </row>
     <row r="467" spans="1:3" ht="21">
       <c r="A467" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B467" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C467" s="1" t="s">
         <v>3</v>
@@ -6990,10 +6990,10 @@
     </row>
     <row r="468" spans="1:3" ht="21">
       <c r="A468" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B468" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C468" s="1" t="s">
         <v>3</v>
@@ -7001,10 +7001,10 @@
     </row>
     <row r="469" spans="1:3" ht="21">
       <c r="A469" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B469" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C469" s="1" t="s">
         <v>3</v>
@@ -7012,10 +7012,10 @@
     </row>
     <row r="470" spans="1:3" ht="21">
       <c r="A470" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B470" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C470" s="1" t="s">
         <v>3</v>
@@ -7023,10 +7023,10 @@
     </row>
     <row r="471" spans="1:3" ht="21">
       <c r="A471" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B471" s="10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C471" s="1" t="s">
         <v>3</v>
@@ -7034,10 +7034,10 @@
     </row>
     <row r="472" spans="1:3" ht="21">
       <c r="A472" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B472" s="10" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C472" s="1" t="s">
         <v>3</v>
@@ -7045,10 +7045,10 @@
     </row>
     <row r="473" spans="1:3" ht="21">
       <c r="A473" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B473" s="10" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C473" s="1" t="s">
         <v>3</v>
@@ -7056,10 +7056,10 @@
     </row>
     <row r="474" spans="1:3" ht="21">
       <c r="A474" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B474" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C474" s="1" t="s">
         <v>3</v>
@@ -7076,10 +7076,10 @@
     </row>
     <row r="477" spans="1:3" ht="21">
       <c r="A477" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B477" s="10" t="s">
         <v>451</v>
-      </c>
-      <c r="B477" s="10" t="s">
-        <v>452</v>
       </c>
       <c r="C477" s="1" t="s">
         <v>3</v>
@@ -7087,10 +7087,10 @@
     </row>
     <row r="478" spans="1:3" ht="21">
       <c r="A478" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B478" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C478" s="1" t="s">
         <v>3</v>
@@ -7098,10 +7098,10 @@
     </row>
     <row r="479" spans="1:3" ht="21">
       <c r="A479" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B479" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C479" s="1" t="s">
         <v>3</v>
@@ -7109,10 +7109,10 @@
     </row>
     <row r="480" spans="1:3" ht="21">
       <c r="A480" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B480" s="10" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C480" s="1" t="s">
         <v>3</v>
@@ -7120,10 +7120,10 @@
     </row>
     <row r="481" spans="1:3" ht="21">
       <c r="A481" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B481" s="10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C481" s="1" t="s">
         <v>3</v>
@@ -7131,10 +7131,10 @@
     </row>
     <row r="482" spans="1:3" ht="21">
       <c r="A482" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B482" s="10" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C482" s="1" t="s">
         <v>3</v>
@@ -7142,10 +7142,10 @@
     </row>
     <row r="483" spans="1:3" ht="21">
       <c r="A483" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B483" s="10" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C483" s="1" t="s">
         <v>3</v>
@@ -7153,10 +7153,10 @@
     </row>
     <row r="484" spans="1:3" ht="21">
       <c r="A484" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B484" s="10" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C484" s="1" t="s">
         <v>3</v>
@@ -7164,10 +7164,10 @@
     </row>
     <row r="485" spans="1:3" ht="21">
       <c r="A485" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B485" s="10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C485" s="1" t="s">
         <v>3</v>
@@ -7175,10 +7175,10 @@
     </row>
     <row r="486" spans="1:3" ht="21">
       <c r="A486" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B486" s="10" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C486" s="1" t="s">
         <v>3</v>
@@ -7498,7 +7498,7 @@
     <hyperlink ref="B323" r:id="rId292"/>
     <hyperlink ref="B324" r:id="rId293"/>
     <hyperlink ref="B325" r:id="rId294"/>
-    <hyperlink ref="B326" r:id="rId295"/>
+    <hyperlink ref="B326" r:id="rId295" display="LRU Cache Implementationa"/>
     <hyperlink ref="B327" r:id="rId296"/>
     <hyperlink ref="B328" r:id="rId297"/>
     <hyperlink ref="B329" r:id="rId298"/>

</xml_diff>

<commit_message>
Added proble status for Arithematic Evaluation Expression problem in SDE Sheet
</commit_message>
<xml_diff>
--- a/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
+++ b/Data Structure & Algorithms/SDE PREPARATION SHEET FOR CODING ROUND.xlsx
@@ -2039,7 +2039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2049,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C319" workbookViewId="0">
-      <selection activeCell="C326" sqref="C326"/>
+    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
+      <selection activeCell="C311" sqref="C311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5321,11 +5321,11 @@
       <c r="A311" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B311" s="10" t="s">
+      <c r="B311" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="C311" s="1" t="s">
-        <v>3</v>
+      <c r="C311" s="8" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="312" spans="1:3" ht="21">

</xml_diff>